<commit_message>
added diagrams (raw forms of it)
</commit_message>
<xml_diff>
--- a/exp5/data/readings.xlsx
+++ b/exp5/data/readings.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="293" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="293" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Tabelle1" sheetId="2" r:id="rId2"/>
+    <sheet name="Dampened oscillations" sheetId="2" r:id="rId2"/>
+    <sheet name="Damp. Osc. Diag" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="22">
   <si>
     <t>Pi</t>
   </si>
@@ -80,6 +80,9 @@
   <si>
     <t>x</t>
   </si>
+  <si>
+    <t>x mean</t>
+  </si>
 </sst>
 </file>
 
@@ -92,12 +95,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -112,8 +121,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -121,6 +131,1313 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="de-CH"/>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>I = 0.65 A</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Dampened oscillations'!$A$7:$A$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.02</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.04</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.06</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.08</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.1199999999999992</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.1399999999999988</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.1599999999999984</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.1799999999999979</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10.199999999999998</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11.219999999999997</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12.239999999999997</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13.259999999999996</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14.279999999999996</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15.299999999999995</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>16.319999999999997</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>17.339999999999996</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>18.359999999999996</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>19.379999999999995</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>20.399999999999995</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>21.419999999999995</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>22.439999999999994</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Dampened oscillations'!$D$7:$D$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.75</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.7749999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.875</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.125</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.22999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8.4999999999999992E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>6.0000000000000005E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="59267712"/>
+        <c:axId val="59266176"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="59267712"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="59266176"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="59266176"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="59267712"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.70000000000000018" r="0.70000000000000018" t="0.78740157499999996" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="de-CH"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-CH"/>
+              <a:t>I = 0.8 A</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>I = 0.8 A</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="log"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Dampened oscillations'!$F$7:$F$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.02</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.04</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.06</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.08</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.1199999999999992</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.1399999999999988</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.1599999999999984</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.1799999999999979</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10.199999999999998</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11.219999999999997</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12.239999999999997</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13.259999999999996</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14.279999999999996</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15.299999999999995</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>16.319999999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Dampened oscillations'!$I$7:$I$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.2750000000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0249999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.125</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.05</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.72499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7.5000000000000011E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.4999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="73737344"/>
+        <c:axId val="73739648"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="73737344"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="73739648"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="73739648"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="73737344"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:legendEntry>
+        <c:idx val="1"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7000000000000004" r="0.7000000000000004" t="0.78740157499999996" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="de-CH"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-CH"/>
+              <a:t>I = 0.5 A</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>I = 0.5 A</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="log"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Dampened oscillations'!$K$7:$K$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="31"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.02</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.04</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.06</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.08</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.1199999999999992</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.1399999999999988</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.1599999999999984</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.1799999999999979</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10.199999999999998</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11.219999999999997</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12.239999999999997</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13.259999999999996</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14.279999999999996</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15.299999999999995</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>16.319999999999997</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>17.339999999999996</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>18.359999999999996</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>19.379999999999995</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>20.399999999999995</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>21.419999999999995</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>22.439999999999994</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>23.459999999999994</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>24.479999999999993</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>25.499999999999993</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>26.519999999999992</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>27.539999999999992</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>28.559999999999992</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>29.579999999999991</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>30.599999999999991</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Dampened oscillations'!$N$7:$N$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="31"/>
+                <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.95</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.375</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.9750000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.5499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.2250000000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.8250000000000002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.1499999999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.97499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.32499999999999996</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.27500000000000002</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.22500000000000001</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.17499999999999999</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.125</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>6.0000000000000005E-2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>3.5000000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="72726400"/>
+        <c:axId val="72727936"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="72726400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="72727936"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="72727936"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="72726400"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:legendEntry>
+        <c:idx val="1"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.70000000000000062" r="0.70000000000000062" t="0.78740157499999996" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="de-CH"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-CH"/>
+              <a:t>I = 0.3 A</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>I = 0.3 A</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="log"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Dampened oscillations'!$P$7:$P$65</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="59"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.02</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.04</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.06</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.08</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.1199999999999992</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.1399999999999988</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.1599999999999984</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.1799999999999979</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10.199999999999998</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11.219999999999997</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12.239999999999997</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13.259999999999996</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14.279999999999996</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15.299999999999995</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>16.319999999999997</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>17.339999999999996</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>18.359999999999996</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>19.379999999999995</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>20.399999999999995</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>21.419999999999995</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>22.439999999999994</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>23.459999999999994</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>24.479999999999993</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>25.499999999999993</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>26.519999999999992</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>27.539999999999992</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>28.559999999999992</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>29.579999999999991</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>30.599999999999991</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>31.61999999999999</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>32.639999999999993</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>33.659999999999997</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>34.68</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>35.700000000000003</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>36.720000000000006</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>37.740000000000009</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>38.760000000000012</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>39.780000000000015</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>40.800000000000018</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>41.820000000000022</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>42.840000000000025</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>43.860000000000028</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>44.880000000000031</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>45.900000000000034</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>46.920000000000037</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>47.94000000000004</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>48.960000000000043</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>49.980000000000047</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>51.00000000000005</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>52.020000000000053</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>53.040000000000056</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>54.060000000000059</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>55.080000000000062</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>56.100000000000065</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>57.120000000000068</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>58.140000000000072</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>59.160000000000075</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Dampened oscillations'!$S$7:$S$65</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="59"/>
+                <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.75</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.625</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.4249999999999998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.8</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.625</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.4500000000000002</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.0249999999999999</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.875</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.7749999999999999</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.625</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.5249999999999999</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.125</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1.125</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.77499999999999991</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.77500000000000002</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.64999999999999991</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.52500000000000002</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.375</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.27500000000000002</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.32499999999999996</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.21000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.15000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.17499999999999999</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.125</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.125</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>8.4999999999999992E-2</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.10500000000000001</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>8.7499999999999994E-2</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="73872128"/>
+        <c:axId val="73874048"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="73872128"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="73874048"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="73874048"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="73872128"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:legendEntry>
+        <c:idx val="1"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.70000000000000062" r="0.70000000000000062" t="0.78740157499999996" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagramm 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Diagramm 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Diagramm 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Diagramm 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1637,98 +2954,114 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O65"/>
+  <dimension ref="A1:S65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="M55" sqref="M55"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:19">
       <c r="A1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:19">
       <c r="A3" t="s">
         <v>17</v>
       </c>
       <c r="B3">
         <v>0.65</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>17</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>0.8</v>
       </c>
-      <c r="I3" t="s">
+      <c r="K3" t="s">
         <v>17</v>
       </c>
-      <c r="J3">
+      <c r="L3">
         <v>0.5</v>
       </c>
-      <c r="M3" t="s">
+      <c r="P3" t="s">
         <v>17</v>
       </c>
-      <c r="N3">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15">
+      <c r="Q3">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
       <c r="A4" t="s">
         <v>18</v>
       </c>
       <c r="B4">
         <v>2.04</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>18</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>2.0659999999999998</v>
       </c>
-      <c r="I4" t="s">
+      <c r="K4" t="s">
         <v>18</v>
       </c>
-      <c r="J4">
+      <c r="L4">
         <v>2.04</v>
       </c>
-      <c r="M4" t="s">
+      <c r="P4" t="s">
         <v>18</v>
       </c>
-      <c r="N4">
+      <c r="Q4">
         <v>2.04</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
-      <c r="A6" t="s">
+    <row r="6" spans="1:19">
+      <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E6" t="s">
+      <c r="C6" s="1"/>
+      <c r="D6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I6" t="s">
+      <c r="H6" s="1"/>
+      <c r="I6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J6" t="s">
+      <c r="L6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="M6" t="s">
+      <c r="M6" s="1"/>
+      <c r="N6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N6" t="s">
+      <c r="Q6" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" spans="1:15">
+      <c r="R6" s="1"/>
+      <c r="S6" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19">
       <c r="A7">
         <f>0</f>
         <v>0</v>
@@ -1739,38 +3072,54 @@
       <c r="C7">
         <v>6</v>
       </c>
-      <c r="E7">
+      <c r="D7">
+        <f>AVERAGE(B7:C7)</f>
+        <v>6</v>
+      </c>
+      <c r="F7">
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="F7">
-        <v>6</v>
-      </c>
       <c r="G7">
         <v>6</v>
       </c>
+      <c r="H7">
+        <v>6</v>
+      </c>
       <c r="I7">
+        <f>AVERAGE(G7:H7)</f>
+        <v>6</v>
+      </c>
+      <c r="K7">
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="J7">
+      <c r="L7">
         <v>6</v>
       </c>
-      <c r="K7">
+      <c r="M7">
         <v>6</v>
       </c>
-      <c r="M7">
+      <c r="N7">
+        <f>AVERAGE(L7:M7)</f>
+        <v>6</v>
+      </c>
+      <c r="P7">
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="N7">
+      <c r="Q7">
         <v>6</v>
       </c>
-      <c r="O7">
+      <c r="R7">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:15">
+      <c r="S7">
+        <f>AVERAGE(Q7:R7)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19">
       <c r="A8">
         <f>A7+$B$4/2</f>
         <v>1.02</v>
@@ -1781,40 +3130,56 @@
       <c r="C8">
         <v>4.7</v>
       </c>
-      <c r="E8">
-        <f>E7+$B$4/2</f>
+      <c r="D8">
+        <f t="shared" ref="D8:D29" si="0">AVERAGE(B8:C8)</f>
+        <v>4.75</v>
+      </c>
+      <c r="F8">
+        <f>F7+$B$4/2</f>
         <v>1.02</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>4.25</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>4.3</v>
       </c>
       <c r="I8">
-        <f>I7+$B$4/2</f>
+        <f t="shared" ref="I8:I23" si="1">AVERAGE(G8:H8)</f>
+        <v>4.2750000000000004</v>
+      </c>
+      <c r="K8">
+        <f>K7+$B$4/2</f>
         <v>1.02</v>
       </c>
-      <c r="J8">
+      <c r="L8">
         <v>5.2</v>
       </c>
-      <c r="K8">
+      <c r="M8">
         <v>5.2</v>
       </c>
-      <c r="M8">
-        <f>M7+$B$4/2</f>
+      <c r="N8">
+        <f t="shared" ref="N8:N37" si="2">AVERAGE(L8:M8)</f>
+        <v>5.2</v>
+      </c>
+      <c r="P8">
+        <f>P7+$B$4/2</f>
         <v>1.02</v>
       </c>
-      <c r="N8">
+      <c r="Q8">
         <v>5.7</v>
       </c>
-      <c r="O8">
+      <c r="R8">
         <v>5.7</v>
       </c>
-    </row>
-    <row r="9" spans="1:15">
+      <c r="S8">
+        <f t="shared" ref="S8:S65" si="3">AVERAGE(Q8:R8)</f>
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19">
       <c r="A9">
-        <f t="shared" ref="A9:A39" si="0">A8+$B$4/2</f>
+        <f t="shared" ref="A9:A29" si="4">A8+$B$4/2</f>
         <v>2.04</v>
       </c>
       <c r="B9">
@@ -1823,40 +3188,56 @@
       <c r="C9">
         <v>3.75</v>
       </c>
-      <c r="E9">
-        <f t="shared" ref="E9:E29" si="1">E8+$B$4/2</f>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>3.7749999999999999</v>
+      </c>
+      <c r="F9">
+        <f t="shared" ref="F9:F23" si="5">F8+$B$4/2</f>
         <v>2.04</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>3</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>3.05</v>
       </c>
       <c r="I9">
-        <f t="shared" ref="I9:I37" si="2">I8+$B$4/2</f>
+        <f t="shared" si="1"/>
+        <v>3.0249999999999999</v>
+      </c>
+      <c r="K9">
+        <f t="shared" ref="K9:K37" si="6">K8+$B$4/2</f>
         <v>2.04</v>
       </c>
-      <c r="J9">
+      <c r="L9">
         <v>4.5</v>
       </c>
-      <c r="K9">
+      <c r="M9">
         <v>4.5</v>
       </c>
-      <c r="M9">
-        <f t="shared" ref="M9:M65" si="3">M8+$B$4/2</f>
+      <c r="N9">
+        <f t="shared" si="2"/>
+        <v>4.5</v>
+      </c>
+      <c r="P9">
+        <f t="shared" ref="P9:P65" si="7">P8+$B$4/2</f>
         <v>2.04</v>
       </c>
-      <c r="N9">
+      <c r="Q9">
         <v>5.3</v>
       </c>
-      <c r="O9">
+      <c r="R9">
         <v>5.2</v>
       </c>
-    </row>
-    <row r="10" spans="1:15">
+      <c r="S9">
+        <f t="shared" si="3"/>
+        <v>5.25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19">
       <c r="A10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>3.06</v>
       </c>
       <c r="B10">
@@ -1865,40 +3246,56 @@
       <c r="C10">
         <v>3</v>
       </c>
-      <c r="E10">
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="5"/>
+        <v>3.06</v>
+      </c>
+      <c r="G10">
+        <v>2.1</v>
+      </c>
+      <c r="H10">
+        <v>2.15</v>
+      </c>
+      <c r="I10">
         <f t="shared" si="1"/>
+        <v>2.125</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="6"/>
         <v>3.06</v>
       </c>
-      <c r="F10">
-        <v>2.1</v>
-      </c>
-      <c r="G10">
-        <v>2.15</v>
-      </c>
-      <c r="I10">
+      <c r="L10">
+        <v>3.95</v>
+      </c>
+      <c r="M10">
+        <v>3.95</v>
+      </c>
+      <c r="N10">
         <f t="shared" si="2"/>
+        <v>3.95</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="7"/>
         <v>3.06</v>
       </c>
-      <c r="J10">
-        <v>3.95</v>
-      </c>
-      <c r="K10">
-        <v>3.95</v>
-      </c>
-      <c r="M10">
-        <f t="shared" si="3"/>
-        <v>3.06</v>
-      </c>
-      <c r="N10">
+      <c r="Q10">
         <v>5</v>
       </c>
-      <c r="O10">
+      <c r="R10">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:15">
+      <c r="S10">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19">
       <c r="A11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>4.08</v>
       </c>
       <c r="B11">
@@ -1907,40 +3304,56 @@
       <c r="C11">
         <v>2.4</v>
       </c>
-      <c r="E11">
-        <f t="shared" si="1"/>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>2.4</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="5"/>
         <v>4.08</v>
-      </c>
-      <c r="F11">
-        <v>1.5</v>
       </c>
       <c r="G11">
         <v>1.5</v>
       </c>
+      <c r="H11">
+        <v>1.5</v>
+      </c>
       <c r="I11">
+        <f t="shared" si="1"/>
+        <v>1.5</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="6"/>
+        <v>4.08</v>
+      </c>
+      <c r="L11">
+        <v>3.35</v>
+      </c>
+      <c r="M11">
+        <v>3.4</v>
+      </c>
+      <c r="N11">
         <f t="shared" si="2"/>
+        <v>3.375</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="7"/>
         <v>4.08</v>
       </c>
-      <c r="J11">
-        <v>3.35</v>
-      </c>
-      <c r="K11">
-        <v>3.4</v>
-      </c>
-      <c r="M11">
-        <f t="shared" si="3"/>
-        <v>4.08</v>
-      </c>
-      <c r="N11">
+      <c r="Q11">
         <v>4.7</v>
       </c>
-      <c r="O11">
+      <c r="R11">
         <v>4.8</v>
       </c>
-    </row>
-    <row r="12" spans="1:15">
+      <c r="S11">
+        <f t="shared" si="3"/>
+        <v>4.75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19">
       <c r="A12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>5.0999999999999996</v>
       </c>
       <c r="B12">
@@ -1949,40 +3362,56 @@
       <c r="C12">
         <v>1.85</v>
       </c>
-      <c r="E12">
-        <f t="shared" si="1"/>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>1.875</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="5"/>
         <v>5.0999999999999996</v>
-      </c>
-      <c r="F12">
-        <v>1.05</v>
       </c>
       <c r="G12">
         <v>1.05</v>
       </c>
+      <c r="H12">
+        <v>1.05</v>
+      </c>
       <c r="I12">
+        <f t="shared" si="1"/>
+        <v>1.05</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="6"/>
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="L12">
+        <v>3</v>
+      </c>
+      <c r="M12">
+        <v>2.95</v>
+      </c>
+      <c r="N12">
         <f t="shared" si="2"/>
+        <v>2.9750000000000001</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="7"/>
         <v>5.0999999999999996</v>
       </c>
-      <c r="J12">
-        <v>3</v>
-      </c>
-      <c r="K12">
-        <v>2.95</v>
-      </c>
-      <c r="M12">
-        <f t="shared" si="3"/>
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="N12">
+      <c r="Q12">
         <v>4.4000000000000004</v>
       </c>
-      <c r="O12">
+      <c r="R12">
         <v>4.4000000000000004</v>
       </c>
-    </row>
-    <row r="13" spans="1:15">
+      <c r="S12">
+        <f t="shared" si="3"/>
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19">
       <c r="A13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>6.1199999999999992</v>
       </c>
       <c r="B13">
@@ -1991,40 +3420,56 @@
       <c r="C13">
         <v>1.5</v>
       </c>
-      <c r="E13">
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="5"/>
+        <v>6.1199999999999992</v>
+      </c>
+      <c r="G13">
+        <v>0.75</v>
+      </c>
+      <c r="H13">
+        <v>0.7</v>
+      </c>
+      <c r="I13">
         <f t="shared" si="1"/>
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="6"/>
         <v>6.1199999999999992</v>
       </c>
-      <c r="F13">
-        <v>0.75</v>
-      </c>
-      <c r="G13">
-        <v>0.7</v>
-      </c>
-      <c r="I13">
+      <c r="L13">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="M13">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="N13">
         <f t="shared" si="2"/>
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="7"/>
         <v>6.1199999999999992</v>
       </c>
-      <c r="J13">
-        <v>2.5499999999999998</v>
-      </c>
-      <c r="K13">
-        <v>2.5499999999999998</v>
-      </c>
-      <c r="M13">
-        <f t="shared" si="3"/>
-        <v>6.1199999999999992</v>
-      </c>
-      <c r="N13">
+      <c r="Q13">
         <v>4.0999999999999996</v>
       </c>
-      <c r="O13">
+      <c r="R13">
         <v>4.0999999999999996</v>
       </c>
-    </row>
-    <row r="14" spans="1:15">
+      <c r="S13">
+        <f t="shared" si="3"/>
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19">
       <c r="A14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>7.1399999999999988</v>
       </c>
       <c r="B14">
@@ -2033,40 +3478,56 @@
       <c r="C14">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E14">
-        <f t="shared" si="1"/>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>1.125</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="5"/>
         <v>7.1399999999999988</v>
-      </c>
-      <c r="F14">
-        <v>0.5</v>
       </c>
       <c r="G14">
         <v>0.5</v>
       </c>
+      <c r="H14">
+        <v>0.5</v>
+      </c>
       <c r="I14">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="6"/>
+        <v>7.1399999999999988</v>
+      </c>
+      <c r="L14">
+        <v>2.25</v>
+      </c>
+      <c r="M14">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="N14">
         <f t="shared" si="2"/>
+        <v>2.2250000000000001</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="7"/>
         <v>7.1399999999999988</v>
       </c>
-      <c r="J14">
-        <v>2.25</v>
-      </c>
-      <c r="K14">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="M14">
-        <f t="shared" si="3"/>
-        <v>7.1399999999999988</v>
-      </c>
-      <c r="N14">
+      <c r="Q14">
         <v>3.9</v>
       </c>
-      <c r="O14">
+      <c r="R14">
         <v>3.9</v>
       </c>
-    </row>
-    <row r="15" spans="1:15">
+      <c r="S14">
+        <f t="shared" si="3"/>
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19">
       <c r="A15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>8.1599999999999984</v>
       </c>
       <c r="B15">
@@ -2075,40 +3536,56 @@
       <c r="C15">
         <v>0.9</v>
       </c>
-      <c r="E15">
-        <f t="shared" si="1"/>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>0.9</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="5"/>
         <v>8.1599999999999984</v>
-      </c>
-      <c r="F15">
-        <v>0.3</v>
       </c>
       <c r="G15">
         <v>0.3</v>
       </c>
+      <c r="H15">
+        <v>0.3</v>
+      </c>
       <c r="I15">
+        <f t="shared" si="1"/>
+        <v>0.3</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="6"/>
+        <v>8.1599999999999984</v>
+      </c>
+      <c r="L15">
+        <v>1.8</v>
+      </c>
+      <c r="M15">
+        <v>1.85</v>
+      </c>
+      <c r="N15">
         <f t="shared" si="2"/>
+        <v>1.8250000000000002</v>
+      </c>
+      <c r="P15">
+        <f t="shared" si="7"/>
         <v>8.1599999999999984</v>
       </c>
-      <c r="J15">
-        <v>1.8</v>
-      </c>
-      <c r="K15">
-        <v>1.85</v>
-      </c>
-      <c r="M15">
-        <f t="shared" si="3"/>
-        <v>8.1599999999999984</v>
-      </c>
-      <c r="N15">
+      <c r="Q15">
         <v>3.6</v>
       </c>
-      <c r="O15">
+      <c r="R15">
         <v>3.65</v>
       </c>
-    </row>
-    <row r="16" spans="1:15">
+      <c r="S15">
+        <f t="shared" si="3"/>
+        <v>3.625</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19">
       <c r="A16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>9.1799999999999979</v>
       </c>
       <c r="B16">
@@ -2117,40 +3594,56 @@
       <c r="C16">
         <v>0.7</v>
       </c>
-      <c r="E16">
-        <f t="shared" si="1"/>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>0.7</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="5"/>
         <v>9.1799999999999979</v>
-      </c>
-      <c r="F16">
-        <v>0.2</v>
       </c>
       <c r="G16">
         <v>0.2</v>
       </c>
+      <c r="H16">
+        <v>0.2</v>
+      </c>
       <c r="I16">
+        <f t="shared" si="1"/>
+        <v>0.2</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="6"/>
+        <v>9.1799999999999979</v>
+      </c>
+      <c r="L16">
+        <v>1.6</v>
+      </c>
+      <c r="M16">
+        <v>1.6</v>
+      </c>
+      <c r="N16">
         <f t="shared" si="2"/>
+        <v>1.6</v>
+      </c>
+      <c r="P16">
+        <f t="shared" si="7"/>
         <v>9.1799999999999979</v>
       </c>
-      <c r="J16">
-        <v>1.6</v>
-      </c>
-      <c r="K16">
-        <v>1.6</v>
-      </c>
-      <c r="M16">
-        <f t="shared" si="3"/>
-        <v>9.1799999999999979</v>
-      </c>
-      <c r="N16">
+      <c r="Q16">
         <v>3.4</v>
       </c>
-      <c r="O16">
+      <c r="R16">
         <v>3.45</v>
       </c>
-    </row>
-    <row r="17" spans="1:15">
+      <c r="S16">
+        <f t="shared" si="3"/>
+        <v>3.4249999999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19">
       <c r="A17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>10.199999999999998</v>
       </c>
       <c r="B17">
@@ -2159,40 +3652,56 @@
       <c r="C17">
         <v>0.55000000000000004</v>
       </c>
-      <c r="E17">
-        <f t="shared" si="1"/>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="5"/>
         <v>10.199999999999998</v>
-      </c>
-      <c r="F17">
-        <v>0.15</v>
       </c>
       <c r="G17">
         <v>0.15</v>
       </c>
+      <c r="H17">
+        <v>0.15</v>
+      </c>
       <c r="I17">
+        <f t="shared" si="1"/>
+        <v>0.15</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="6"/>
+        <v>10.199999999999998</v>
+      </c>
+      <c r="L17">
+        <v>1.2</v>
+      </c>
+      <c r="M17">
+        <v>1.4</v>
+      </c>
+      <c r="N17">
         <f t="shared" si="2"/>
+        <v>1.2999999999999998</v>
+      </c>
+      <c r="P17">
+        <f t="shared" si="7"/>
         <v>10.199999999999998</v>
       </c>
-      <c r="J17">
-        <v>1.2</v>
-      </c>
-      <c r="K17">
-        <v>1.4</v>
-      </c>
-      <c r="M17">
-        <f t="shared" si="3"/>
-        <v>10.199999999999998</v>
-      </c>
-      <c r="N17">
+      <c r="Q17">
         <v>3.2</v>
       </c>
-      <c r="O17">
+      <c r="R17">
         <v>3.2</v>
       </c>
-    </row>
-    <row r="18" spans="1:15">
+      <c r="S17">
+        <f t="shared" si="3"/>
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19">
       <c r="A18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>11.219999999999997</v>
       </c>
       <c r="B18">
@@ -2201,40 +3710,56 @@
       <c r="C18">
         <v>0.4</v>
       </c>
-      <c r="E18">
-        <f t="shared" si="1"/>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>0.4</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="5"/>
         <v>11.219999999999997</v>
-      </c>
-      <c r="F18">
-        <v>0.1</v>
       </c>
       <c r="G18">
         <v>0.1</v>
       </c>
+      <c r="H18">
+        <v>0.1</v>
+      </c>
       <c r="I18">
+        <f t="shared" si="1"/>
+        <v>0.1</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="6"/>
+        <v>11.219999999999997</v>
+      </c>
+      <c r="L18">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="M18">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="N18">
         <f t="shared" si="2"/>
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="P18">
+        <f t="shared" si="7"/>
         <v>11.219999999999997</v>
       </c>
-      <c r="J18">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="K18">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="M18">
-        <f t="shared" si="3"/>
-        <v>11.219999999999997</v>
-      </c>
-      <c r="N18">
+      <c r="Q18">
         <v>3</v>
       </c>
-      <c r="O18">
+      <c r="R18">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="1:15">
+      <c r="S18">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19">
       <c r="A19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>12.239999999999997</v>
       </c>
       <c r="B19">
@@ -2243,40 +3768,56 @@
       <c r="C19">
         <v>0.3</v>
       </c>
-      <c r="E19">
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>0.3</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="5"/>
+        <v>12.239999999999997</v>
+      </c>
+      <c r="G19">
+        <v>0.08</v>
+      </c>
+      <c r="H19">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="I19">
         <f t="shared" si="1"/>
+        <v>7.5000000000000011E-2</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="6"/>
         <v>12.239999999999997</v>
       </c>
-      <c r="F19">
-        <v>0.08</v>
-      </c>
-      <c r="G19">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="I19">
+      <c r="L19">
+        <v>0.95</v>
+      </c>
+      <c r="M19">
+        <v>1</v>
+      </c>
+      <c r="N19">
         <f t="shared" si="2"/>
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="P19">
+        <f t="shared" si="7"/>
         <v>12.239999999999997</v>
       </c>
-      <c r="J19">
-        <v>0.95</v>
-      </c>
-      <c r="K19">
-        <v>1</v>
-      </c>
-      <c r="M19">
-        <f t="shared" si="3"/>
-        <v>12.239999999999997</v>
-      </c>
-      <c r="N19">
+      <c r="Q19">
         <v>2.8</v>
       </c>
-      <c r="O19">
+      <c r="R19">
         <v>2.8</v>
       </c>
-    </row>
-    <row r="20" spans="1:15">
+      <c r="S19">
+        <f t="shared" si="3"/>
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19">
       <c r="A20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>13.259999999999996</v>
       </c>
       <c r="B20">
@@ -2285,40 +3826,56 @@
       <c r="C20">
         <v>0.21</v>
       </c>
-      <c r="E20">
-        <f t="shared" si="1"/>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>0.22999999999999998</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="5"/>
         <v>13.259999999999996</v>
-      </c>
-      <c r="F20">
-        <v>0.05</v>
       </c>
       <c r="G20">
         <v>0.05</v>
       </c>
+      <c r="H20">
+        <v>0.05</v>
+      </c>
       <c r="I20">
+        <f t="shared" si="1"/>
+        <v>0.05</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="6"/>
+        <v>13.259999999999996</v>
+      </c>
+      <c r="L20">
+        <v>0.85</v>
+      </c>
+      <c r="M20">
+        <v>0.75</v>
+      </c>
+      <c r="N20">
         <f t="shared" si="2"/>
+        <v>0.8</v>
+      </c>
+      <c r="P20">
+        <f t="shared" si="7"/>
         <v>13.259999999999996</v>
       </c>
-      <c r="J20">
-        <v>0.85</v>
-      </c>
-      <c r="K20">
-        <v>0.75</v>
-      </c>
-      <c r="M20">
-        <f t="shared" si="3"/>
-        <v>13.259999999999996</v>
-      </c>
-      <c r="N20">
+      <c r="Q20">
         <v>2.6</v>
       </c>
-      <c r="O20">
+      <c r="R20">
         <v>2.65</v>
       </c>
-    </row>
-    <row r="21" spans="1:15">
+      <c r="S20">
+        <f t="shared" si="3"/>
+        <v>2.625</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19">
       <c r="A21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>14.279999999999996</v>
       </c>
       <c r="B21">
@@ -2327,40 +3884,56 @@
       <c r="C21">
         <v>0.2</v>
       </c>
-      <c r="E21">
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="5"/>
+        <v>14.279999999999996</v>
+      </c>
+      <c r="G21">
+        <v>0.01</v>
+      </c>
+      <c r="H21">
+        <v>0.02</v>
+      </c>
+      <c r="I21">
         <f t="shared" si="1"/>
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="6"/>
         <v>14.279999999999996</v>
       </c>
-      <c r="F21">
-        <v>0.01</v>
-      </c>
-      <c r="G21">
-        <v>0.02</v>
-      </c>
-      <c r="I21">
+      <c r="L21">
+        <v>0.65</v>
+      </c>
+      <c r="M21">
+        <v>0.75</v>
+      </c>
+      <c r="N21">
         <f t="shared" si="2"/>
+        <v>0.7</v>
+      </c>
+      <c r="P21">
+        <f t="shared" si="7"/>
         <v>14.279999999999996</v>
       </c>
-      <c r="J21">
-        <v>0.65</v>
-      </c>
-      <c r="K21">
-        <v>0.75</v>
-      </c>
-      <c r="M21">
-        <f t="shared" si="3"/>
-        <v>14.279999999999996</v>
-      </c>
-      <c r="N21">
+      <c r="Q21">
         <v>2.4</v>
       </c>
-      <c r="O21">
+      <c r="R21">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="22" spans="1:15">
+      <c r="S21">
+        <f t="shared" si="3"/>
+        <v>2.4500000000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19">
       <c r="A22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>15.299999999999995</v>
       </c>
       <c r="B22">
@@ -2369,40 +3942,56 @@
       <c r="C22">
         <v>0.15</v>
       </c>
-      <c r="E22">
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>0.15</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="5"/>
+        <v>15.299999999999995</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0.02</v>
+      </c>
+      <c r="I22">
         <f t="shared" si="1"/>
+        <v>0.01</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="6"/>
         <v>15.299999999999995</v>
       </c>
-      <c r="F22">
-        <v>0</v>
-      </c>
-      <c r="G22">
-        <v>0.02</v>
-      </c>
-      <c r="I22">
+      <c r="L22">
+        <v>0.6</v>
+      </c>
+      <c r="M22">
+        <v>0.5</v>
+      </c>
+      <c r="N22">
         <f t="shared" si="2"/>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="P22">
+        <f t="shared" si="7"/>
         <v>15.299999999999995</v>
       </c>
-      <c r="J22">
-        <v>0.6</v>
-      </c>
-      <c r="K22">
-        <v>0.5</v>
-      </c>
-      <c r="M22">
-        <f t="shared" si="3"/>
-        <v>15.299999999999995</v>
-      </c>
-      <c r="N22">
+      <c r="Q22">
         <v>2.2999999999999998</v>
       </c>
-      <c r="O22">
+      <c r="R22">
         <v>2.2999999999999998</v>
       </c>
-    </row>
-    <row r="23" spans="1:15">
+      <c r="S22">
+        <f t="shared" si="3"/>
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19">
       <c r="A23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>16.319999999999997</v>
       </c>
       <c r="B23">
@@ -2411,40 +4000,56 @@
       <c r="C23">
         <v>0.1</v>
       </c>
-      <c r="E23">
-        <f t="shared" si="1"/>
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="5"/>
         <v>16.319999999999997</v>
-      </c>
-      <c r="F23">
-        <v>0</v>
       </c>
       <c r="G23">
         <v>0</v>
       </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
       <c r="I23">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="6"/>
+        <v>16.319999999999997</v>
+      </c>
+      <c r="L23">
+        <v>0.45</v>
+      </c>
+      <c r="M23">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="N23">
         <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+      <c r="P23">
+        <f t="shared" si="7"/>
         <v>16.319999999999997</v>
       </c>
-      <c r="J23">
-        <v>0.45</v>
-      </c>
-      <c r="K23">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="M23">
-        <f t="shared" si="3"/>
-        <v>16.319999999999997</v>
-      </c>
-      <c r="N23">
+      <c r="Q23">
         <v>2.2000000000000002</v>
       </c>
-      <c r="O23">
+      <c r="R23">
         <v>2.2000000000000002</v>
       </c>
-    </row>
-    <row r="24" spans="1:15">
+      <c r="S23">
+        <f t="shared" si="3"/>
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19">
       <c r="A24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>17.339999999999996</v>
       </c>
       <c r="B24">
@@ -2453,30 +4058,42 @@
       <c r="C24">
         <v>0.09</v>
       </c>
-      <c r="I24">
+      <c r="D24">
+        <f t="shared" si="0"/>
+        <v>8.4999999999999992E-2</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="6"/>
+        <v>17.339999999999996</v>
+      </c>
+      <c r="L24">
+        <v>0.45</v>
+      </c>
+      <c r="M24">
+        <v>0.45</v>
+      </c>
+      <c r="N24">
         <f t="shared" si="2"/>
+        <v>0.45</v>
+      </c>
+      <c r="P24">
+        <f t="shared" si="7"/>
         <v>17.339999999999996</v>
       </c>
-      <c r="J24">
-        <v>0.45</v>
-      </c>
-      <c r="K24">
-        <v>0.45</v>
-      </c>
-      <c r="M24">
-        <f t="shared" si="3"/>
-        <v>17.339999999999996</v>
-      </c>
-      <c r="N24">
+      <c r="Q24">
         <v>2</v>
       </c>
-      <c r="O24">
+      <c r="R24">
         <v>2.0499999999999998</v>
       </c>
-    </row>
-    <row r="25" spans="1:15">
+      <c r="S24">
+        <f t="shared" si="3"/>
+        <v>2.0249999999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19">
       <c r="A25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>18.359999999999996</v>
       </c>
       <c r="B25">
@@ -2485,28 +4102,40 @@
       <c r="C25">
         <v>0.05</v>
       </c>
-      <c r="I25">
+      <c r="D25">
+        <f t="shared" si="0"/>
+        <v>6.0000000000000005E-2</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="6"/>
+        <v>18.359999999999996</v>
+      </c>
+      <c r="L25">
+        <v>0.3</v>
+      </c>
+      <c r="M25">
+        <v>0.35</v>
+      </c>
+      <c r="N25">
         <f t="shared" si="2"/>
+        <v>0.32499999999999996</v>
+      </c>
+      <c r="P25">
+        <f t="shared" si="7"/>
         <v>18.359999999999996</v>
       </c>
-      <c r="J25">
-        <v>0.3</v>
-      </c>
-      <c r="K25">
-        <v>0.35</v>
-      </c>
-      <c r="M25">
-        <f t="shared" si="3"/>
-        <v>18.359999999999996</v>
-      </c>
-      <c r="N25">
+      <c r="Q25">
         <v>1.85</v>
       </c>
-      <c r="O25">
+      <c r="R25">
         <v>1.9</v>
       </c>
-    </row>
-    <row r="26" spans="1:15">
+      <c r="S25">
+        <f t="shared" si="3"/>
+        <v>1.875</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19">
       <c r="A26">
         <f>A25+$B$4/2</f>
         <v>19.379999999999995</v>
@@ -2517,30 +4146,42 @@
       <c r="C26">
         <v>0.05</v>
       </c>
-      <c r="I26">
+      <c r="D26">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="6"/>
+        <v>19.379999999999995</v>
+      </c>
+      <c r="L26">
+        <v>0.3</v>
+      </c>
+      <c r="M26">
+        <v>0.25</v>
+      </c>
+      <c r="N26">
         <f t="shared" si="2"/>
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="P26">
+        <f t="shared" si="7"/>
         <v>19.379999999999995</v>
       </c>
-      <c r="J26">
-        <v>0.3</v>
-      </c>
-      <c r="K26">
-        <v>0.25</v>
-      </c>
-      <c r="M26">
-        <f t="shared" si="3"/>
-        <v>19.379999999999995</v>
-      </c>
-      <c r="N26">
+      <c r="Q26">
         <v>1.8</v>
       </c>
-      <c r="O26">
+      <c r="R26">
         <v>1.75</v>
       </c>
-    </row>
-    <row r="27" spans="1:15">
+      <c r="S26">
+        <f t="shared" si="3"/>
+        <v>1.7749999999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19">
       <c r="A27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>20.399999999999995</v>
       </c>
       <c r="B27">
@@ -2549,30 +4190,42 @@
       <c r="C27">
         <v>0.02</v>
       </c>
-      <c r="I27">
+      <c r="D27">
+        <f t="shared" si="0"/>
+        <v>0.02</v>
+      </c>
+      <c r="K27">
+        <f t="shared" si="6"/>
+        <v>20.399999999999995</v>
+      </c>
+      <c r="L27">
+        <v>0.2</v>
+      </c>
+      <c r="M27">
+        <v>0.25</v>
+      </c>
+      <c r="N27">
         <f t="shared" si="2"/>
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="P27">
+        <f t="shared" si="7"/>
         <v>20.399999999999995</v>
       </c>
-      <c r="J27">
-        <v>0.2</v>
-      </c>
-      <c r="K27">
-        <v>0.25</v>
-      </c>
-      <c r="M27">
-        <f t="shared" si="3"/>
-        <v>20.399999999999995</v>
-      </c>
-      <c r="N27">
+      <c r="Q27">
         <v>1.6</v>
       </c>
-      <c r="O27">
+      <c r="R27">
         <v>1.65</v>
       </c>
-    </row>
-    <row r="28" spans="1:15">
+      <c r="S27">
+        <f t="shared" si="3"/>
+        <v>1.625</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19">
       <c r="A28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>21.419999999999995</v>
       </c>
       <c r="B28">
@@ -2581,30 +4234,42 @@
       <c r="C28">
         <v>0.03</v>
       </c>
-      <c r="I28">
+      <c r="D28">
+        <f t="shared" si="0"/>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="K28">
+        <f t="shared" si="6"/>
+        <v>21.419999999999995</v>
+      </c>
+      <c r="L28">
+        <v>0.2</v>
+      </c>
+      <c r="M28">
+        <v>0.15</v>
+      </c>
+      <c r="N28">
         <f t="shared" si="2"/>
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="P28">
+        <f t="shared" si="7"/>
         <v>21.419999999999995</v>
       </c>
-      <c r="J28">
-        <v>0.2</v>
-      </c>
-      <c r="K28">
-        <v>0.15</v>
-      </c>
-      <c r="M28">
-        <f t="shared" si="3"/>
-        <v>21.419999999999995</v>
-      </c>
-      <c r="N28">
+      <c r="Q28">
         <v>1.5</v>
       </c>
-      <c r="O28">
+      <c r="R28">
         <v>1.55</v>
       </c>
-    </row>
-    <row r="29" spans="1:15">
+      <c r="S28">
+        <f t="shared" si="3"/>
+        <v>1.5249999999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19">
       <c r="A29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>22.439999999999994</v>
       </c>
       <c r="B29">
@@ -2613,540 +4278,744 @@
       <c r="C29">
         <v>0</v>
       </c>
-      <c r="I29">
+      <c r="D29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K29">
+        <f t="shared" si="6"/>
+        <v>22.439999999999994</v>
+      </c>
+      <c r="L29">
+        <v>0.15</v>
+      </c>
+      <c r="M29">
+        <v>0.15</v>
+      </c>
+      <c r="N29">
         <f t="shared" si="2"/>
+        <v>0.15</v>
+      </c>
+      <c r="P29">
+        <f t="shared" si="7"/>
         <v>22.439999999999994</v>
       </c>
-      <c r="J29">
+      <c r="Q29">
+        <v>1.4</v>
+      </c>
+      <c r="R29">
+        <v>1.4</v>
+      </c>
+      <c r="S29">
+        <f t="shared" si="3"/>
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19">
+      <c r="K30">
+        <f t="shared" si="6"/>
+        <v>23.459999999999994</v>
+      </c>
+      <c r="L30">
         <v>0.15</v>
       </c>
-      <c r="K29">
+      <c r="M30">
+        <v>0.1</v>
+      </c>
+      <c r="N30">
+        <f t="shared" si="2"/>
+        <v>0.125</v>
+      </c>
+      <c r="P30">
+        <f t="shared" si="7"/>
+        <v>23.459999999999994</v>
+      </c>
+      <c r="Q30">
+        <v>1.3</v>
+      </c>
+      <c r="R30">
+        <v>1.3</v>
+      </c>
+      <c r="S30">
+        <f t="shared" si="3"/>
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19">
+      <c r="K31">
+        <f t="shared" si="6"/>
+        <v>24.479999999999993</v>
+      </c>
+      <c r="L31">
+        <v>0.1</v>
+      </c>
+      <c r="M31">
+        <v>0.1</v>
+      </c>
+      <c r="N31">
+        <f t="shared" si="2"/>
+        <v>0.1</v>
+      </c>
+      <c r="P31">
+        <f t="shared" si="7"/>
+        <v>24.479999999999993</v>
+      </c>
+      <c r="Q31">
+        <v>1.2</v>
+      </c>
+      <c r="R31">
+        <v>1.2</v>
+      </c>
+      <c r="S31">
+        <f t="shared" si="3"/>
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19">
+      <c r="K32">
+        <f t="shared" si="6"/>
+        <v>25.499999999999993</v>
+      </c>
+      <c r="L32">
+        <v>0.1</v>
+      </c>
+      <c r="M32">
+        <v>0.08</v>
+      </c>
+      <c r="N32">
+        <f t="shared" si="2"/>
+        <v>0.09</v>
+      </c>
+      <c r="P32">
+        <f t="shared" si="7"/>
+        <v>25.499999999999993</v>
+      </c>
+      <c r="Q32">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="R32">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="S32">
+        <f t="shared" si="3"/>
+        <v>1.125</v>
+      </c>
+    </row>
+    <row r="33" spans="11:19">
+      <c r="K33">
+        <f t="shared" si="6"/>
+        <v>26.519999999999992</v>
+      </c>
+      <c r="L33">
+        <v>0.05</v>
+      </c>
+      <c r="M33">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="N33">
+        <f t="shared" si="2"/>
+        <v>6.0000000000000005E-2</v>
+      </c>
+      <c r="P33">
+        <f t="shared" si="7"/>
+        <v>26.519999999999992</v>
+      </c>
+      <c r="Q33">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="R33">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="S33">
+        <f t="shared" si="3"/>
+        <v>1.125</v>
+      </c>
+    </row>
+    <row r="34" spans="11:19">
+      <c r="K34">
+        <f t="shared" si="6"/>
+        <v>27.539999999999992</v>
+      </c>
+      <c r="L34">
+        <v>0.02</v>
+      </c>
+      <c r="M34">
+        <v>0.05</v>
+      </c>
+      <c r="N34">
+        <f t="shared" si="2"/>
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="P34">
+        <f t="shared" si="7"/>
+        <v>27.539999999999992</v>
+      </c>
+      <c r="Q34">
+        <v>0.9</v>
+      </c>
+      <c r="R34">
+        <v>1</v>
+      </c>
+      <c r="S34">
+        <f t="shared" si="3"/>
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="35" spans="11:19">
+      <c r="K35">
+        <f t="shared" si="6"/>
+        <v>28.559999999999992</v>
+      </c>
+      <c r="L35">
+        <v>0.02</v>
+      </c>
+      <c r="M35">
+        <v>0.02</v>
+      </c>
+      <c r="N35">
+        <f t="shared" si="2"/>
+        <v>0.02</v>
+      </c>
+      <c r="P35">
+        <f t="shared" si="7"/>
+        <v>28.559999999999992</v>
+      </c>
+      <c r="Q35">
+        <v>0.9</v>
+      </c>
+      <c r="R35">
+        <v>0.9</v>
+      </c>
+      <c r="S35">
+        <f t="shared" si="3"/>
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="36" spans="11:19">
+      <c r="K36">
+        <f t="shared" si="6"/>
+        <v>29.579999999999991</v>
+      </c>
+      <c r="L36">
+        <v>0.03</v>
+      </c>
+      <c r="M36">
+        <v>0.02</v>
+      </c>
+      <c r="N36">
+        <f t="shared" si="2"/>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="P36">
+        <f t="shared" si="7"/>
+        <v>29.579999999999991</v>
+      </c>
+      <c r="Q36">
+        <v>0.7</v>
+      </c>
+      <c r="R36">
+        <v>0.85</v>
+      </c>
+      <c r="S36">
+        <f t="shared" si="3"/>
+        <v>0.77499999999999991</v>
+      </c>
+    </row>
+    <row r="37" spans="11:19">
+      <c r="K37">
+        <f t="shared" si="6"/>
+        <v>30.599999999999991</v>
+      </c>
+      <c r="L37">
+        <v>0</v>
+      </c>
+      <c r="M37">
+        <v>0</v>
+      </c>
+      <c r="N37">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P37">
+        <f t="shared" si="7"/>
+        <v>30.599999999999991</v>
+      </c>
+      <c r="Q37">
+        <v>0.75</v>
+      </c>
+      <c r="R37">
+        <v>0.8</v>
+      </c>
+      <c r="S37">
+        <f t="shared" si="3"/>
+        <v>0.77500000000000002</v>
+      </c>
+    </row>
+    <row r="38" spans="11:19">
+      <c r="P38">
+        <f t="shared" si="7"/>
+        <v>31.61999999999999</v>
+      </c>
+      <c r="Q38">
+        <v>0.6</v>
+      </c>
+      <c r="R38">
+        <v>0.7</v>
+      </c>
+      <c r="S38">
+        <f t="shared" si="3"/>
+        <v>0.64999999999999991</v>
+      </c>
+    </row>
+    <row r="39" spans="11:19">
+      <c r="P39">
+        <f t="shared" si="7"/>
+        <v>32.639999999999993</v>
+      </c>
+      <c r="Q39">
+        <v>0.65</v>
+      </c>
+      <c r="R39">
+        <v>0.65</v>
+      </c>
+      <c r="S39">
+        <f t="shared" si="3"/>
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="40" spans="11:19">
+      <c r="P40">
+        <f t="shared" si="7"/>
+        <v>33.659999999999997</v>
+      </c>
+      <c r="Q40">
+        <v>0.45</v>
+      </c>
+      <c r="R40">
+        <v>0.6</v>
+      </c>
+      <c r="S40">
+        <f t="shared" si="3"/>
+        <v>0.52500000000000002</v>
+      </c>
+    </row>
+    <row r="41" spans="11:19">
+      <c r="P41">
+        <f t="shared" si="7"/>
+        <v>34.68</v>
+      </c>
+      <c r="Q41">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="R41">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="S41">
+        <f t="shared" si="3"/>
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="42" spans="11:19">
+      <c r="P42">
+        <f t="shared" si="7"/>
+        <v>35.700000000000003</v>
+      </c>
+      <c r="Q42">
+        <v>0.4</v>
+      </c>
+      <c r="R42">
+        <v>0.5</v>
+      </c>
+      <c r="S42">
+        <f t="shared" si="3"/>
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="43" spans="11:19">
+      <c r="P43">
+        <f t="shared" si="7"/>
+        <v>36.720000000000006</v>
+      </c>
+      <c r="Q43">
+        <v>0.45</v>
+      </c>
+      <c r="R43">
+        <v>0.45</v>
+      </c>
+      <c r="S43">
+        <f t="shared" si="3"/>
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="44" spans="11:19">
+      <c r="P44">
+        <f t="shared" si="7"/>
+        <v>37.740000000000009</v>
+      </c>
+      <c r="Q44">
+        <v>0.3</v>
+      </c>
+      <c r="R44">
+        <v>0.45</v>
+      </c>
+      <c r="S44">
+        <f t="shared" si="3"/>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="45" spans="11:19">
+      <c r="P45">
+        <f t="shared" si="7"/>
+        <v>38.760000000000012</v>
+      </c>
+      <c r="Q45">
+        <v>0.4</v>
+      </c>
+      <c r="R45">
+        <v>0.4</v>
+      </c>
+      <c r="S45">
+        <f t="shared" si="3"/>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="46" spans="11:19">
+      <c r="P46">
+        <f t="shared" si="7"/>
+        <v>39.780000000000015</v>
+      </c>
+      <c r="Q46">
+        <v>0.2</v>
+      </c>
+      <c r="R46">
+        <v>0.35</v>
+      </c>
+      <c r="S46">
+        <f t="shared" si="3"/>
+        <v>0.27500000000000002</v>
+      </c>
+    </row>
+    <row r="47" spans="11:19">
+      <c r="P47">
+        <f t="shared" si="7"/>
+        <v>40.800000000000018</v>
+      </c>
+      <c r="Q47">
+        <v>0.3</v>
+      </c>
+      <c r="R47">
+        <v>0.35</v>
+      </c>
+      <c r="S47">
+        <f t="shared" si="3"/>
+        <v>0.32499999999999996</v>
+      </c>
+    </row>
+    <row r="48" spans="11:19">
+      <c r="P48">
+        <f t="shared" si="7"/>
+        <v>41.820000000000022</v>
+      </c>
+      <c r="Q48">
+        <v>0.2</v>
+      </c>
+      <c r="R48">
+        <v>0.3</v>
+      </c>
+      <c r="S48">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="49" spans="16:19">
+      <c r="P49">
+        <f t="shared" si="7"/>
+        <v>42.840000000000025</v>
+      </c>
+      <c r="Q49">
+        <v>0.25</v>
+      </c>
+      <c r="R49">
+        <v>0.25</v>
+      </c>
+      <c r="S49">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="50" spans="16:19">
+      <c r="P50">
+        <f t="shared" si="7"/>
+        <v>43.860000000000028</v>
+      </c>
+      <c r="Q50">
         <v>0.15</v>
       </c>
-      <c r="M29">
-        <f t="shared" si="3"/>
-        <v>22.439999999999994</v>
-      </c>
-      <c r="N29">
-        <v>1.4</v>
-      </c>
-      <c r="O29">
-        <v>1.4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15">
-      <c r="I30">
-        <f t="shared" si="2"/>
-        <v>23.459999999999994</v>
-      </c>
-      <c r="J30">
+      <c r="R50">
+        <v>0.25</v>
+      </c>
+      <c r="S50">
+        <f t="shared" si="3"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="51" spans="16:19">
+      <c r="P51">
+        <f t="shared" si="7"/>
+        <v>44.880000000000031</v>
+      </c>
+      <c r="Q51">
+        <v>0.2</v>
+      </c>
+      <c r="R51">
+        <v>0.22</v>
+      </c>
+      <c r="S51">
+        <f t="shared" si="3"/>
+        <v>0.21000000000000002</v>
+      </c>
+    </row>
+    <row r="52" spans="16:19">
+      <c r="P52">
+        <f t="shared" si="7"/>
+        <v>45.900000000000034</v>
+      </c>
+      <c r="Q52">
+        <v>0.1</v>
+      </c>
+      <c r="R52">
+        <v>0.2</v>
+      </c>
+      <c r="S52">
+        <f t="shared" si="3"/>
+        <v>0.15000000000000002</v>
+      </c>
+    </row>
+    <row r="53" spans="16:19">
+      <c r="P53">
+        <f t="shared" si="7"/>
+        <v>46.920000000000037</v>
+      </c>
+      <c r="Q53">
         <v>0.15</v>
       </c>
-      <c r="K30">
+      <c r="R53">
+        <v>0.2</v>
+      </c>
+      <c r="S53">
+        <f t="shared" si="3"/>
+        <v>0.17499999999999999</v>
+      </c>
+    </row>
+    <row r="54" spans="16:19">
+      <c r="P54">
+        <f t="shared" si="7"/>
+        <v>47.94000000000004</v>
+      </c>
+      <c r="Q54">
         <v>0.1</v>
       </c>
-      <c r="M30">
-        <f t="shared" si="3"/>
-        <v>23.459999999999994</v>
-      </c>
-      <c r="N30">
-        <v>1.3</v>
-      </c>
-      <c r="O30">
-        <v>1.3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15">
-      <c r="I31">
-        <f t="shared" si="2"/>
-        <v>24.479999999999993</v>
-      </c>
-      <c r="J31">
+      <c r="R54">
+        <v>0.15</v>
+      </c>
+      <c r="S54">
+        <f t="shared" si="3"/>
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="55" spans="16:19">
+      <c r="P55">
+        <f t="shared" si="7"/>
+        <v>48.960000000000043</v>
+      </c>
+      <c r="Q55">
         <v>0.1</v>
       </c>
-      <c r="K31">
+      <c r="R55">
+        <v>0.15</v>
+      </c>
+      <c r="S55">
+        <f t="shared" si="3"/>
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="56" spans="16:19">
+      <c r="P56">
+        <f t="shared" si="7"/>
+        <v>49.980000000000047</v>
+      </c>
+      <c r="Q56">
+        <v>0.05</v>
+      </c>
+      <c r="R56">
+        <v>0.12</v>
+      </c>
+      <c r="S56">
+        <f t="shared" si="3"/>
+        <v>8.4999999999999992E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="16:19">
+      <c r="P57">
+        <f t="shared" si="7"/>
+        <v>51.00000000000005</v>
+      </c>
+      <c r="Q57">
         <v>0.1</v>
       </c>
-      <c r="M31">
-        <f t="shared" si="3"/>
-        <v>24.479999999999993</v>
-      </c>
-      <c r="N31">
-        <v>1.2</v>
-      </c>
-      <c r="O31">
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15">
-      <c r="I32">
-        <f t="shared" si="2"/>
-        <v>25.499999999999993</v>
-      </c>
-      <c r="J32">
+      <c r="R57">
+        <v>0.11</v>
+      </c>
+      <c r="S57">
+        <f t="shared" si="3"/>
+        <v>0.10500000000000001</v>
+      </c>
+    </row>
+    <row r="58" spans="16:19">
+      <c r="P58">
+        <f t="shared" si="7"/>
+        <v>52.020000000000053</v>
+      </c>
+      <c r="Q58">
+        <v>0</v>
+      </c>
+      <c r="R58">
         <v>0.1</v>
       </c>
-      <c r="K32">
+      <c r="S58">
+        <f t="shared" si="3"/>
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="59" spans="16:19">
+      <c r="P59">
+        <f t="shared" si="7"/>
+        <v>53.040000000000056</v>
+      </c>
+      <c r="Q59">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="R59">
+        <v>0.1</v>
+      </c>
+      <c r="S59">
+        <f t="shared" si="3"/>
+        <v>8.7499999999999994E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="16:19">
+      <c r="P60">
+        <f t="shared" si="7"/>
+        <v>54.060000000000059</v>
+      </c>
+      <c r="Q60">
+        <v>0</v>
+      </c>
+      <c r="R60">
         <v>0.08</v>
       </c>
-      <c r="M32">
-        <f t="shared" si="3"/>
-        <v>25.499999999999993</v>
-      </c>
-      <c r="N32">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="O32">
-        <v>1.1499999999999999</v>
-      </c>
-    </row>
-    <row r="33" spans="9:15">
-      <c r="I33">
-        <f t="shared" si="2"/>
-        <v>26.519999999999992</v>
-      </c>
-      <c r="J33">
+      <c r="S60">
+        <f t="shared" si="3"/>
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="61" spans="16:19">
+      <c r="P61">
+        <f t="shared" si="7"/>
+        <v>55.080000000000062</v>
+      </c>
+      <c r="Q61">
         <v>0.05</v>
       </c>
-      <c r="K33">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="M33">
-        <f t="shared" si="3"/>
-        <v>26.519999999999992</v>
-      </c>
-      <c r="N33">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="O33">
-        <v>1.1499999999999999</v>
-      </c>
-    </row>
-    <row r="34" spans="9:15">
-      <c r="I34">
-        <f t="shared" si="2"/>
-        <v>27.539999999999992</v>
-      </c>
-      <c r="J34">
-        <v>0.02</v>
-      </c>
-      <c r="K34">
+      <c r="R61">
         <v>0.05</v>
       </c>
-      <c r="M34">
-        <f t="shared" si="3"/>
-        <v>27.539999999999992</v>
-      </c>
-      <c r="N34">
-        <v>0.9</v>
-      </c>
-      <c r="O34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="9:15">
-      <c r="I35">
-        <f t="shared" si="2"/>
-        <v>28.559999999999992</v>
-      </c>
-      <c r="J35">
-        <v>0.02</v>
-      </c>
-      <c r="K35">
-        <v>0.02</v>
-      </c>
-      <c r="M35">
-        <f t="shared" si="3"/>
-        <v>28.559999999999992</v>
-      </c>
-      <c r="N35">
-        <v>0.9</v>
-      </c>
-      <c r="O35">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="36" spans="9:15">
-      <c r="I36">
-        <f t="shared" si="2"/>
-        <v>29.579999999999991</v>
-      </c>
-      <c r="J36">
-        <v>0.03</v>
-      </c>
-      <c r="K36">
-        <v>0.02</v>
-      </c>
-      <c r="M36">
-        <f t="shared" si="3"/>
-        <v>29.579999999999991</v>
-      </c>
-      <c r="N36">
-        <v>0.7</v>
-      </c>
-      <c r="O36">
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="37" spans="9:15">
-      <c r="I37">
-        <f t="shared" si="2"/>
-        <v>30.599999999999991</v>
-      </c>
-      <c r="J37">
+      <c r="S61">
+        <f t="shared" si="3"/>
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="62" spans="16:19">
+      <c r="P62">
+        <f t="shared" si="7"/>
+        <v>56.100000000000065</v>
+      </c>
+      <c r="Q62">
         <v>0</v>
       </c>
-      <c r="K37">
+      <c r="R62">
+        <v>0.05</v>
+      </c>
+      <c r="S62">
+        <f t="shared" si="3"/>
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="16:19">
+      <c r="P63">
+        <f t="shared" si="7"/>
+        <v>57.120000000000068</v>
+      </c>
+      <c r="Q63">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="R63">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="S63">
+        <f t="shared" si="3"/>
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="64" spans="16:19">
+      <c r="P64">
+        <f t="shared" si="7"/>
+        <v>58.140000000000072</v>
+      </c>
+      <c r="Q64">
         <v>0</v>
       </c>
-      <c r="M37">
-        <f t="shared" si="3"/>
-        <v>30.599999999999991</v>
-      </c>
-      <c r="N37">
-        <v>0.75</v>
-      </c>
-      <c r="O37">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="38" spans="9:15">
-      <c r="M38">
-        <f t="shared" si="3"/>
-        <v>31.61999999999999</v>
-      </c>
-      <c r="N38">
-        <v>0.6</v>
-      </c>
-      <c r="O38">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="39" spans="9:15">
-      <c r="M39">
-        <f t="shared" si="3"/>
-        <v>32.639999999999993</v>
-      </c>
-      <c r="N39">
-        <v>0.65</v>
-      </c>
-      <c r="O39">
-        <v>0.65</v>
-      </c>
-    </row>
-    <row r="40" spans="9:15">
-      <c r="M40">
-        <f t="shared" si="3"/>
-        <v>33.659999999999997</v>
-      </c>
-      <c r="N40">
-        <v>0.45</v>
-      </c>
-      <c r="O40">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="41" spans="9:15">
-      <c r="M41">
-        <f t="shared" si="3"/>
-        <v>34.68</v>
-      </c>
-      <c r="N41">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="O41">
-        <v>0.55000000000000004</v>
-      </c>
-    </row>
-    <row r="42" spans="9:15">
-      <c r="M42">
-        <f t="shared" si="3"/>
-        <v>35.700000000000003</v>
-      </c>
-      <c r="N42">
-        <v>0.4</v>
-      </c>
-      <c r="O42">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="43" spans="9:15">
-      <c r="M43">
-        <f t="shared" si="3"/>
-        <v>36.720000000000006</v>
-      </c>
-      <c r="N43">
-        <v>0.45</v>
-      </c>
-      <c r="O43">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="44" spans="9:15">
-      <c r="M44">
-        <f t="shared" si="3"/>
-        <v>37.740000000000009</v>
-      </c>
-      <c r="N44">
-        <v>0.3</v>
-      </c>
-      <c r="O44">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="45" spans="9:15">
-      <c r="M45">
-        <f t="shared" si="3"/>
-        <v>38.760000000000012</v>
-      </c>
-      <c r="N45">
-        <v>0.4</v>
-      </c>
-      <c r="O45">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="46" spans="9:15">
-      <c r="M46">
-        <f t="shared" si="3"/>
-        <v>39.780000000000015</v>
-      </c>
-      <c r="N46">
-        <v>0.2</v>
-      </c>
-      <c r="O46">
-        <v>0.35</v>
-      </c>
-    </row>
-    <row r="47" spans="9:15">
-      <c r="M47">
-        <f t="shared" si="3"/>
-        <v>40.800000000000018</v>
-      </c>
-      <c r="N47">
-        <v>0.3</v>
-      </c>
-      <c r="O47">
-        <v>0.35</v>
-      </c>
-    </row>
-    <row r="48" spans="9:15">
-      <c r="M48">
-        <f t="shared" si="3"/>
-        <v>41.820000000000022</v>
-      </c>
-      <c r="N48">
-        <v>0.2</v>
-      </c>
-      <c r="O48">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="49" spans="13:15">
-      <c r="M49">
-        <f t="shared" si="3"/>
-        <v>42.840000000000025</v>
-      </c>
-      <c r="N49">
-        <v>0.25</v>
-      </c>
-      <c r="O49">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="50" spans="13:15">
-      <c r="M50">
-        <f t="shared" si="3"/>
-        <v>43.860000000000028</v>
-      </c>
-      <c r="N50">
-        <v>0.15</v>
-      </c>
-      <c r="O50">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="51" spans="13:15">
-      <c r="M51">
-        <f t="shared" si="3"/>
-        <v>44.880000000000031</v>
-      </c>
-      <c r="N51">
-        <v>0.2</v>
-      </c>
-      <c r="O51">
-        <v>0.22</v>
-      </c>
-    </row>
-    <row r="52" spans="13:15">
-      <c r="M52">
-        <f t="shared" si="3"/>
-        <v>45.900000000000034</v>
-      </c>
-      <c r="N52">
-        <v>0.1</v>
-      </c>
-      <c r="O52">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="53" spans="13:15">
-      <c r="M53">
-        <f t="shared" si="3"/>
-        <v>46.920000000000037</v>
-      </c>
-      <c r="N53">
-        <v>0.15</v>
-      </c>
-      <c r="O53">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="54" spans="13:15">
-      <c r="M54">
-        <f t="shared" si="3"/>
-        <v>47.94000000000004</v>
-      </c>
-      <c r="N54">
-        <v>0.1</v>
-      </c>
-      <c r="O54">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="55" spans="13:15">
-      <c r="M55">
-        <f t="shared" si="3"/>
-        <v>48.960000000000043</v>
-      </c>
-      <c r="N55">
-        <v>0.1</v>
-      </c>
-      <c r="O55">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="56" spans="13:15">
-      <c r="M56">
-        <f t="shared" si="3"/>
-        <v>49.980000000000047</v>
-      </c>
-      <c r="N56">
-        <v>0.05</v>
-      </c>
-      <c r="O56">
-        <v>0.12</v>
-      </c>
-    </row>
-    <row r="57" spans="13:15">
-      <c r="M57">
-        <f t="shared" si="3"/>
-        <v>51.00000000000005</v>
-      </c>
-      <c r="N57">
-        <v>0.1</v>
-      </c>
-      <c r="O57">
-        <v>0.11</v>
-      </c>
-    </row>
-    <row r="58" spans="13:15">
-      <c r="M58">
-        <f t="shared" si="3"/>
-        <v>52.020000000000053</v>
-      </c>
-      <c r="N58">
+      <c r="R64">
         <v>0</v>
       </c>
-      <c r="O58">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="59" spans="13:15">
-      <c r="M59">
-        <f t="shared" si="3"/>
-        <v>53.040000000000056</v>
-      </c>
-      <c r="N59">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="O59">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="60" spans="13:15">
-      <c r="M60">
-        <f t="shared" si="3"/>
-        <v>54.060000000000059</v>
-      </c>
-      <c r="N60">
+      <c r="S64">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="O60">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="61" spans="13:15">
-      <c r="M61">
-        <f t="shared" si="3"/>
-        <v>55.080000000000062</v>
-      </c>
-      <c r="N61">
-        <v>0.05</v>
-      </c>
-      <c r="O61">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="62" spans="13:15">
-      <c r="M62">
-        <f t="shared" si="3"/>
-        <v>56.100000000000065</v>
-      </c>
-      <c r="N62">
+    </row>
+    <row r="65" spans="16:19">
+      <c r="P65">
+        <f t="shared" si="7"/>
+        <v>59.160000000000075</v>
+      </c>
+      <c r="Q65">
         <v>0</v>
       </c>
-      <c r="O62">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="63" spans="13:15">
-      <c r="M63">
-        <f t="shared" si="3"/>
-        <v>57.120000000000068</v>
-      </c>
-      <c r="N63">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="O63">
-        <v>2.5000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="64" spans="13:15">
-      <c r="M64">
-        <f t="shared" si="3"/>
-        <v>58.140000000000072</v>
-      </c>
-      <c r="N64">
+      <c r="R65">
         <v>0</v>
       </c>
-      <c r="O64">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="13:15">
-      <c r="M65">
-        <f t="shared" si="3"/>
-        <v>59.160000000000075</v>
-      </c>
-      <c r="N65">
-        <v>0</v>
-      </c>
-      <c r="O65">
+      <c r="S65">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="N20" sqref="N20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added trend lines to diagrams
</commit_message>
<xml_diff>
--- a/exp5/data/readings.xlsx
+++ b/exp5/data/readings.xlsx
@@ -155,12 +155,26 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="exp"/>
+            <c:intercept val="6"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.26521500437445317"/>
+                  <c:y val="1.1883931175269758E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Dampened oscillations'!$A$7:$A$29</c:f>
+              <c:f>'Dampened oscillations'!$A$7:$A$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="23"/>
+                <c:ptCount val="22"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -226,19 +240,16 @@
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>21.419999999999995</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>22.439999999999994</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Dampened oscillations'!$D$7:$D$29</c:f>
+              <c:f>'Dampened oscillations'!$D$7:$D$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="23"/>
+                <c:ptCount val="22"/>
                 <c:pt idx="0">
                   <c:v>6</c:v>
                 </c:pt>
@@ -304,31 +315,28 @@
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>2.5000000000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="59267712"/>
-        <c:axId val="59266176"/>
+        <c:axId val="85972096"/>
+        <c:axId val="85973632"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="59267712"/>
+        <c:axId val="85972096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="59266176"/>
+        <c:crossAx val="85973632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="59266176"/>
+        <c:axId val="85973632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -336,7 +344,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="59267712"/>
+        <c:crossAx val="85972096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -349,7 +357,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.70000000000000018" r="0.70000000000000018" t="0.78740157499999996" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.78740157499999996" l="0.70000000000000029" r="0.70000000000000029" t="0.78740157499999996" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -395,12 +403,26 @@
           <c:trendline>
             <c:trendlineType val="log"/>
           </c:trendline>
+          <c:trendline>
+            <c:trendlineType val="exp"/>
+            <c:intercept val="6"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.33003543307086614"/>
+                  <c:y val="-8.0708661417322834E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Dampened oscillations'!$F$7:$F$23</c:f>
+              <c:f>'Dampened oscillations'!$F$7:$F$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -448,19 +470,16 @@
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>15.299999999999995</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>16.319999999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Dampened oscillations'!$I$7:$I$23</c:f>
+              <c:f>'Dampened oscillations'!$I$7:$I$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>6</c:v>
                 </c:pt>
@@ -508,31 +527,28 @@
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>0.01</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="73737344"/>
-        <c:axId val="73739648"/>
+        <c:axId val="85547648"/>
+        <c:axId val="85569920"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="73737344"/>
+        <c:axId val="85547648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73739648"/>
+        <c:crossAx val="85569920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="73739648"/>
+        <c:axId val="85569920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -540,7 +556,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73737344"/>
+        <c:crossAx val="85547648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -557,7 +573,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.7000000000000004" r="0.7000000000000004" t="0.78740157499999996" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.78740157499999996" l="0.70000000000000051" r="0.70000000000000051" t="0.78740157499999996" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -603,12 +619,26 @@
           <c:trendline>
             <c:trendlineType val="log"/>
           </c:trendline>
+          <c:trendline>
+            <c:trendlineType val="exp"/>
+            <c:intercept val="6"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.40212445319335083"/>
+                  <c:y val="1.5077282006415865E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Dampened oscillations'!$K$7:$K$37</c:f>
+              <c:f>'Dampened oscillations'!$K$7:$K$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="31"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -698,19 +728,16 @@
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>29.579999999999991</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>30.599999999999991</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Dampened oscillations'!$N$7:$N$37</c:f>
+              <c:f>'Dampened oscillations'!$N$7:$N$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="31"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>6</c:v>
                 </c:pt>
@@ -800,31 +827,28 @@
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>2.5000000000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="72726400"/>
-        <c:axId val="72727936"/>
+        <c:axId val="86058112"/>
+        <c:axId val="86059648"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="72726400"/>
+        <c:axId val="86058112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72727936"/>
+        <c:crossAx val="86059648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="72727936"/>
+        <c:axId val="86059648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -832,7 +856,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72726400"/>
+        <c:crossAx val="86058112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -895,12 +919,26 @@
           <c:trendline>
             <c:trendlineType val="log"/>
           </c:trendline>
+          <c:trendline>
+            <c:trendlineType val="exp"/>
+            <c:intercept val="6"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.22591972878390201"/>
+                  <c:y val="1.5077282006415865E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Dampened oscillations'!$P$7:$P$65</c:f>
+              <c:f>'Dampened oscillations'!$P$7:$P$63</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="59"/>
+                <c:ptCount val="57"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1071,22 +1109,16 @@
                 </c:pt>
                 <c:pt idx="56">
                   <c:v>57.120000000000068</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>58.140000000000072</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>59.160000000000075</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Dampened oscillations'!$S$7:$S$65</c:f>
+              <c:f>'Dampened oscillations'!$S$7:$S$63</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="59"/>
+                <c:ptCount val="57"/>
                 <c:pt idx="0">
                   <c:v>6</c:v>
                 </c:pt>
@@ -1257,34 +1289,28 @@
                 </c:pt>
                 <c:pt idx="56">
                   <c:v>2.5000000000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="73872128"/>
-        <c:axId val="73874048"/>
+        <c:axId val="86080896"/>
+        <c:axId val="86107264"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="73872128"/>
+        <c:axId val="86080896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73874048"/>
+        <c:crossAx val="86107264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="73874048"/>
+        <c:axId val="86107264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1292,7 +1318,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73872128"/>
+        <c:crossAx val="86080896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2956,8 +2982,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S65"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14"/>
+    <sheetView topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -5010,7 +5036,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+      <selection activeCell="N33" sqref="N33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>

</xml_diff>

<commit_message>
changed y-axis to log
</commit_message>
<xml_diff>
--- a/exp5/data/readings.xlsx
+++ b/exp5/data/readings.xlsx
@@ -162,8 +162,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.26521500437445317"/>
-                  <c:y val="1.1883931175269758E-3"/>
+                  <c:x val="0.26521500437445322"/>
+                  <c:y val="1.1883931175269763E-3"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -320,31 +320,32 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="85972096"/>
-        <c:axId val="85973632"/>
+        <c:axId val="80075008"/>
+        <c:axId val="79900672"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="85972096"/>
+        <c:axId val="80075008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85973632"/>
+        <c:crossAx val="79900672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="85973632"/>
+        <c:axId val="79900672"/>
         <c:scaling>
+          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85972096"/>
+        <c:crossAx val="80075008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -357,7 +358,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.70000000000000029" r="0.70000000000000029" t="0.78740157499999996" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.78740157499999996" l="0.7000000000000004" r="0.7000000000000004" t="0.78740157499999996" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -410,8 +411,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.33003543307086614"/>
-                  <c:y val="-8.0708661417322834E-3"/>
+                  <c:x val="0.33003543307086625"/>
+                  <c:y val="-8.0708661417322851E-3"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -532,31 +533,32 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="85547648"/>
-        <c:axId val="85569920"/>
+        <c:axId val="79933824"/>
+        <c:axId val="79935360"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="85547648"/>
+        <c:axId val="79933824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85569920"/>
+        <c:crossAx val="79935360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="85569920"/>
+        <c:axId val="79935360"/>
         <c:scaling>
+          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85547648"/>
+        <c:crossAx val="79933824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -573,7 +575,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.70000000000000051" r="0.70000000000000051" t="0.78740157499999996" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.78740157499999996" l="0.70000000000000062" r="0.70000000000000062" t="0.78740157499999996" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -626,8 +628,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.40212445319335083"/>
-                  <c:y val="1.5077282006415865E-2"/>
+                  <c:x val="0.40212445319335088"/>
+                  <c:y val="1.5077282006415864E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -832,31 +834,32 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="86058112"/>
-        <c:axId val="86059648"/>
+        <c:axId val="80424320"/>
+        <c:axId val="80434304"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="86058112"/>
+        <c:axId val="80424320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86059648"/>
+        <c:crossAx val="80434304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="86059648"/>
+        <c:axId val="80434304"/>
         <c:scaling>
+          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86058112"/>
+        <c:crossAx val="80424320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -927,7 +930,7 @@
               <c:layout>
                 <c:manualLayout>
                   <c:x val="0.22591972878390201"/>
-                  <c:y val="1.5077282006415865E-2"/>
+                  <c:y val="1.5077282006415864E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -1294,31 +1297,32 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="86080896"/>
-        <c:axId val="86107264"/>
+        <c:axId val="80476800"/>
+        <c:axId val="80556416"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="86080896"/>
+        <c:axId val="80476800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86107264"/>
+        <c:crossAx val="80556416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="86107264"/>
+        <c:axId val="80556416"/>
         <c:scaling>
+          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86080896"/>
+        <c:crossAx val="80476800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5035,7 +5039,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="N33" sqref="N33"/>
     </sheetView>
   </sheetViews>

</xml_diff>